<commit_message>
Added jars needed for Calander page and a few other changes.
</commit_message>
<xml_diff>
--- a/journal_entries.xlsx
+++ b/journal_entries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>2023-10-07</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>here is another test</t>
+  </si>
+  <si>
+    <t>2023-10-09</t>
+  </si>
+  <si>
+    <t>This is a title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entry </t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -161,6 +170,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
created path to logo, updated method for excel spreadsheet
</commit_message>
<xml_diff>
--- a/journal_entries.xlsx
+++ b/journal_entries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>2023-10-07</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t xml:space="preserve">Entry </t>
+  </si>
+  <si>
+    <t>2023-11-05</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -181,6 +187,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Everything now resets on the Journal Page once the save button is hit.
</commit_message>
<xml_diff>
--- a/journal_entries.xlsx
+++ b/journal_entries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>2023-10-07</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>2023-12-05</t>
+  </si>
+  <si>
+    <t>Final Test of rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TnjThis is the final test to see if everything resets. </t>
+  </si>
+  <si>
+    <t>images/1701834132599</t>
+  </si>
+  <si>
+    <t>Stressed</t>
   </si>
 </sst>
 </file>
@@ -104,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -198,6 +213,23 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>